<commit_message>
Update link between variables in modules
</commit_message>
<xml_diff>
--- a/documentation/modules/Variablesandmodules.xlsx
+++ b/documentation/modules/Variablesandmodules.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$160</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$154</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="59">
   <si>
     <t>CONS_H_T_V(prd,regg): household consumption on aggregated product</t>
   </si>
@@ -90,9 +90,6 @@
     <t>INTER_USE_T_V(prd,regg,ind): use of intermediate inputs on aggregated product level</t>
   </si>
   <si>
-    <t>VA_V(regg,ind): use of aggregated production factors</t>
-  </si>
-  <si>
     <t>KL_V(reg,va,regg,ind): use of specific production factors</t>
   </si>
   <si>
@@ -141,18 +138,12 @@
     <t>EXPORT_ROW_V(reg,prd): export to the rest of the world regions</t>
   </si>
   <si>
-    <t>SV_ROW_V(prd,regg): stock changes of rest of the world products</t>
-  </si>
-  <si>
     <t>Trade</t>
   </si>
   <si>
     <t>Production</t>
   </si>
   <si>
-    <t>KLS_V(reg,va): Production of production factors</t>
-  </si>
-  <si>
     <t>GDPDEF_V: GDP deflator used as numeraire</t>
   </si>
   <si>
@@ -195,13 +186,16 @@
     <t>GDPCUR_V(regg): GDP in current prices (value)</t>
   </si>
   <si>
-    <t>PVA_V(regg,ind): aggregate production factors price</t>
-  </si>
-  <si>
     <t>PIMP_MOD_V(prd,regg): aggregate imported product price for the aggregate imported from modeled regions</t>
   </si>
   <si>
     <t>PIMP_T_V(prd,regg): aggregate total imported product price</t>
+  </si>
+  <si>
+    <t>PnKL_V(regg,ind): aggregate production factors price</t>
+  </si>
+  <si>
+    <t>nKL_V(regg,ind): use of aggregated production factors</t>
   </si>
 </sst>
 </file>
@@ -540,11 +534,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D160"/>
+  <dimension ref="A1:D154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -563,7 +555,7 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -574,7 +566,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -588,7 +580,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -602,7 +594,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -616,7 +608,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -630,7 +622,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -644,7 +636,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -658,7 +650,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -672,7 +664,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -686,7 +678,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -700,10 +692,10 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -714,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -728,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -742,10 +734,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -756,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -770,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -784,7 +776,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -798,7 +790,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -812,7 +804,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -826,10 +818,10 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -840,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -854,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -868,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -882,7 +874,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -896,7 +888,7 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -910,7 +902,7 @@
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -924,7 +916,7 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -938,7 +930,7 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -952,7 +944,7 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -966,7 +958,7 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -980,7 +972,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -994,7 +986,7 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1008,7 +1000,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1022,7 +1014,7 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1036,7 +1028,7 @@
         <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1050,7 +1042,7 @@
         <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1064,7 +1056,7 @@
         <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1078,7 +1070,7 @@
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1092,7 +1084,7 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -1106,7 +1098,7 @@
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1120,7 +1112,7 @@
         <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1134,7 +1126,7 @@
         <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1148,7 +1140,7 @@
         <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1162,7 +1154,7 @@
         <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -1176,7 +1168,7 @@
         <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1190,7 +1182,7 @@
         <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -1204,7 +1196,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1218,7 +1210,7 @@
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -1232,7 +1224,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1240,10 +1232,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C50" t="s">
         <v>19</v>
@@ -1254,13 +1246,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1268,13 +1260,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -1282,10 +1274,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C53" t="s">
         <v>19</v>
@@ -1296,13 +1288,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -1310,13 +1302,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C55" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -1324,10 +1316,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C56" t="s">
         <v>19</v>
@@ -1338,27 +1330,27 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C57" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C58" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -1366,10 +1358,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" t="s">
         <v>45</v>
-      </c>
-      <c r="B59" t="s">
-        <v>48</v>
       </c>
       <c r="C59" t="s">
         <v>19</v>
@@ -1380,13 +1372,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" t="s">
         <v>45</v>
       </c>
-      <c r="B60" t="s">
-        <v>48</v>
-      </c>
       <c r="C60" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -1394,13 +1386,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" t="s">
         <v>45</v>
       </c>
-      <c r="B61" t="s">
-        <v>48</v>
-      </c>
       <c r="C61" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -1408,10 +1400,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B62" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C62" t="s">
         <v>19</v>
@@ -1422,27 +1414,27 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C63" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B64" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C64" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -1450,10 +1442,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B65" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C65" t="s">
         <v>19</v>
@@ -1464,27 +1456,27 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B66" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C67" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -1492,10 +1484,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C68" t="s">
         <v>19</v>
@@ -1506,27 +1498,27 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B69" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C69" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B70" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C70" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -1534,10 +1526,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B71" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C71" t="s">
         <v>19</v>
@@ -1548,13 +1540,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B72" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C72" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -1562,13 +1554,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B73" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C73" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -1576,10 +1568,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B74" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C74" t="s">
         <v>19</v>
@@ -1590,13 +1582,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B75" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C75" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -1604,13 +1596,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B76" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C76" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -1618,10 +1610,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B77" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C77" t="s">
         <v>19</v>
@@ -1632,27 +1624,27 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B78" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C78" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B79" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C79" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -1660,10 +1652,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B80" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C80" t="s">
         <v>19</v>
@@ -1674,27 +1666,27 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B81" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C81" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B82" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C82" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -1702,10 +1694,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B83" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C83" t="s">
         <v>19</v>
@@ -1716,13 +1708,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B84" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C84" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -1730,13 +1722,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B85" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C85" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -1744,10 +1736,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B86" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C86" t="s">
         <v>19</v>
@@ -1758,13 +1750,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B87" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C87" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -1772,13 +1764,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B88" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C88" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -1786,10 +1778,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B89" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C89" t="s">
         <v>19</v>
@@ -1800,13 +1792,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B90" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C90" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -1814,13 +1806,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B91" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C91" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -1828,7 +1820,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B92" t="s">
         <v>22</v>
@@ -1842,13 +1834,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B93" t="s">
         <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -1856,13 +1848,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B94" t="s">
         <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -1870,10 +1862,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B95" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C95" t="s">
         <v>19</v>
@@ -1884,13 +1876,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B96" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C96" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -1898,13 +1890,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B97" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C97" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -1912,10 +1904,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B98" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C98" t="s">
         <v>19</v>
@@ -1926,13 +1918,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B99" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C99" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -1940,24 +1932,24 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B100" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C100" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B101" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C101" t="s">
         <v>19</v>
@@ -1968,27 +1960,27 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B102" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C102" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B103" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C103" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -1996,41 +1988,41 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B104" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C104" t="s">
         <v>19</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B105" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C105" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B106" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C106" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -2038,27 +2030,27 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B107" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C107" t="s">
         <v>19</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B108" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C108" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -2066,24 +2058,24 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B109" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C109" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B110" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C110" t="s">
         <v>19</v>
@@ -2094,13 +2086,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B111" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C111" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -2108,24 +2100,24 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B112" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C112" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B113" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C113" t="s">
         <v>19</v>
@@ -2136,35 +2128,35 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B114" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C114" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B115" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C115" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B116" t="s">
         <v>30</v>
@@ -2178,27 +2170,27 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B117" t="s">
         <v>30</v>
       </c>
       <c r="C117" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B118" t="s">
         <v>30</v>
       </c>
       <c r="C118" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D118">
         <v>1</v>
@@ -2206,10 +2198,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B119" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C119" t="s">
         <v>19</v>
@@ -2220,27 +2212,27 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B120" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C120" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B121" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C121" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D121">
         <v>1</v>
@@ -2248,7 +2240,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B122" t="s">
         <v>28</v>
@@ -2262,27 +2254,27 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B123" t="s">
         <v>28</v>
       </c>
       <c r="C123" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B124" t="s">
         <v>28</v>
       </c>
       <c r="C124" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D124">
         <v>1</v>
@@ -2290,10 +2282,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B125" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C125" t="s">
         <v>19</v>
@@ -2304,27 +2296,27 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B126" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C126" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B127" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C127" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D127">
         <v>1</v>
@@ -2332,10 +2324,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B128" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C128" t="s">
         <v>19</v>
@@ -2346,13 +2338,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B129" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C129" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -2360,13 +2352,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B130" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C130" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -2374,7 +2366,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B131" t="s">
         <v>32</v>
@@ -2388,27 +2380,27 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B132" t="s">
         <v>32</v>
       </c>
       <c r="C132" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D132">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B133" t="s">
         <v>32</v>
       </c>
       <c r="C133" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D133">
         <v>1</v>
@@ -2416,10 +2408,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B134" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C134" t="s">
         <v>19</v>
@@ -2430,13 +2422,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B135" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C135" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D135">
         <v>0</v>
@@ -2444,21 +2436,21 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B136" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C136" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D136">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B137" t="s">
         <v>36</v>
@@ -2472,13 +2464,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B138" t="s">
         <v>36</v>
       </c>
       <c r="C138" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D138">
         <v>0</v>
@@ -2486,13 +2478,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B139" t="s">
         <v>36</v>
       </c>
       <c r="C139" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D139">
         <v>1</v>
@@ -2500,10 +2492,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B140" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C140" t="s">
         <v>19</v>
@@ -2514,13 +2506,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B141" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C141" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -2528,24 +2520,24 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B142" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C142" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D142">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B143" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C143" t="s">
         <v>19</v>
@@ -2556,27 +2548,27 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B144" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C144" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D144">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B145" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C145" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D145">
         <v>1</v>
@@ -2584,7 +2576,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B146" t="s">
         <v>26</v>
@@ -2598,27 +2590,27 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B147" t="s">
         <v>26</v>
       </c>
       <c r="C147" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D147">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B148" t="s">
         <v>26</v>
       </c>
       <c r="C148" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D148">
         <v>1</v>
@@ -2626,41 +2618,41 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B149" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C149" t="s">
         <v>19</v>
       </c>
       <c r="D149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B150" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C150" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D150">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B151" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C151" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D151">
         <v>1</v>
@@ -2668,27 +2660,27 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B152" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C152" t="s">
         <v>19</v>
       </c>
       <c r="D152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B153" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C153" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D153">
         <v>1</v>
@@ -2696,100 +2688,16 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B154" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C154" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D154">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>41</v>
-      </c>
-      <c r="B155" t="s">
-        <v>34</v>
-      </c>
-      <c r="C155" t="s">
-        <v>19</v>
-      </c>
-      <c r="D155">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>41</v>
-      </c>
-      <c r="B156" t="s">
-        <v>34</v>
-      </c>
-      <c r="C156" t="s">
-        <v>42</v>
-      </c>
-      <c r="D156">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>41</v>
-      </c>
-      <c r="B157" t="s">
-        <v>34</v>
-      </c>
-      <c r="C157" t="s">
-        <v>45</v>
-      </c>
-      <c r="D157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>41</v>
-      </c>
-      <c r="B158" t="s">
-        <v>38</v>
-      </c>
-      <c r="C158" t="s">
-        <v>19</v>
-      </c>
-      <c r="D158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>41</v>
-      </c>
-      <c r="B159" t="s">
-        <v>38</v>
-      </c>
-      <c r="C159" t="s">
-        <v>42</v>
-      </c>
-      <c r="D159">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>41</v>
-      </c>
-      <c r="B160" t="s">
-        <v>38</v>
-      </c>
-      <c r="C160" t="s">
-        <v>45</v>
-      </c>
-      <c r="D160">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2797,6 +2705,7 @@
     <sortCondition ref="A2:A160"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>